<commit_message>
fix: :zap: Mayor Refactor change TFIDF and SVM Linear into manual
</commit_message>
<xml_diff>
--- a/docs/TFIDF-2.xlsx
+++ b/docs/TFIDF-2.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\000-Python-Project\ran-svm\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5A099D8-D116-40B1-BA70-540E8A1A4583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407B9C11-C2B7-48FC-85B7-F5DAA0917D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D7AEF1D6-F98F-43C5-A90D-6E0604E616FC}"/>
   </bookViews>
   <sheets>
     <sheet name="train_metrics" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1025,7 +1038,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
"Refactored TextClassifier and added TFIDFVectorizer class; updated predict function and added ModelManager class; changed train_metrics.csv and trained_model.pkl files"
</commit_message>
<xml_diff>
--- a/docs/TFIDF-2.xlsx
+++ b/docs/TFIDF-2.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\000-Python-Project\ran-svm\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5A099D8-D116-40B1-BA70-540E8A1A4583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C958AC-26DE-4B50-8C72-4184B9E0079F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D7AEF1D6-F98F-43C5-A90D-6E0604E616FC}"/>
   </bookViews>
   <sheets>
     <sheet name="train_metrics" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
   <si>
     <t>Terms</t>
   </si>
@@ -122,7 +135,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,6 +269,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -632,7 +654,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -647,6 +669,8 @@
     <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1022,10 +1046,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{705A8970-8CB4-48B2-B3D5-7512ACB6F527}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="R18" sqref="R18:S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,9 +1060,10 @@
     <col min="6" max="6" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1067,7 +1092,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1101,8 +1126,14 @@
         <f>ROUND(E2*$G2,3)</f>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2">
+        <v>0.23076792961122999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1136,8 +1167,14 @@
         <f t="shared" ref="I3:I23" si="5">ROUND(E3*$G3,3)</f>
         <v>0.14099999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O3" t="s">
+        <v>10</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -1171,8 +1208,14 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1206,8 +1249,14 @@
         <f t="shared" si="5"/>
         <v>0.14099999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -1241,8 +1290,14 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O6" t="s">
+        <v>13</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -1276,8 +1331,14 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O7" t="s">
+        <v>14</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -1311,8 +1372,14 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O8" t="s">
+        <v>15</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1346,8 +1413,14 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O9" t="s">
+        <v>16</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -1381,8 +1454,14 @@
         <f t="shared" si="5"/>
         <v>0.14099999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O10" t="s">
+        <v>17</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -1416,8 +1495,14 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O11" t="s">
+        <v>18</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -1451,8 +1536,14 @@
         <f t="shared" si="5"/>
         <v>0.14099999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O12" t="s">
+        <v>19</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -1486,8 +1577,14 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O13" t="s">
+        <v>20</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -1521,8 +1618,14 @@
         <f t="shared" si="5"/>
         <v>0.14099999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O14" t="s">
+        <v>21</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -1556,8 +1659,14 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O15" t="s">
+        <v>22</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -1591,8 +1700,14 @@
         <f t="shared" si="5"/>
         <v>0.14099999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O16" t="s">
+        <v>23</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
@@ -1626,8 +1741,14 @@
         <f t="shared" si="5"/>
         <v>0.14099999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O17" t="s">
+        <v>24</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>25</v>
       </c>
@@ -1661,8 +1782,15 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O18" t="s">
+        <v>25</v>
+      </c>
+      <c r="P18">
+        <v>0.97300881941683603</v>
+      </c>
+      <c r="R18" s="7"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
@@ -1696,8 +1824,14 @@
         <f t="shared" si="5"/>
         <v>0.14099999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O19" t="s">
+        <v>26</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>27</v>
       </c>
@@ -1731,8 +1865,14 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O20" t="s">
+        <v>27</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>28</v>
       </c>
@@ -1766,8 +1906,14 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O21" t="s">
+        <v>28</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>29</v>
       </c>
@@ -1801,8 +1947,14 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O22" t="s">
+        <v>29</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>30</v>
       </c>
@@ -1836,8 +1988,14 @@
         <f t="shared" si="5"/>
         <v>0.14099999999999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O23" t="s">
+        <v>30</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -1851,6 +2009,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>